<commit_message>
Started writing the velocity matching rule.  Test currently fails.  Live with it.
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>b1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,6 +66,18 @@
   </si>
   <si>
     <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>avg velocity excluding b2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -236,16 +248,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -588,23 +600,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="B1" t="s">
         <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -614,8 +632,18 @@
       <c r="C2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <f ca="1">RANDBETWEEN(0, 5)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -625,8 +653,18 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <f ca="1">RANDBETWEEN(0, 5)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -636,8 +674,18 @@
       <c r="C4">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <f ca="1">RANDBETWEEN(0, 5)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -647,13 +695,50 @@
       <c r="C5">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f ca="1">RANDBETWEEN(0, 5)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="F6">
+        <f ca="1">RANDBETWEEN(0, 5)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <f ca="1">RANDBETWEEN(0, 5)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="B8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8">
+        <f>(D2+D4+D5)/3</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="E8">
+        <f>(E2+E4+E5)/3</f>
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <f ca="1">RANDBETWEEN(0, 5)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -662,7 +747,7 @@
         <v>1.4142135623730951</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -671,7 +756,7 @@
         <v>1.5811388300841898</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -680,12 +765,12 @@
         <v>8.6023252670426267</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:6">
       <c r="B13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -698,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -740,7 +825,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>